<commit_message>
Added info to the page to give context. Replaced data to represent only Active units.
</commit_message>
<xml_diff>
--- a/scripts/output_data/summary_tax_values_plus_unit_counts.xlsx
+++ b/scripts/output_data/summary_tax_values_plus_unit_counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humph\Documents\Github\housing-preservation\scripts\output_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humph\Documents\Github\housing-insights\scripts\output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="summary_tax_values" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -265,11 +265,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -711,9 +709,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -756,59 +753,57 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1123,7 +1118,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,37 +1192,37 @@
         <v>75</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>22</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2">
         <v>217017080</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2">
         <v>563652910</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>223728280</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2">
         <v>705756700</v>
       </c>
       <c r="K2" t="s">
         <v>76</v>
       </c>
       <c r="L2">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="M2">
         <v>10169467</v>
@@ -1271,16 +1266,16 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3">
         <v>83834560</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3">
         <v>234166020</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3">
         <v>87894470</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3">
         <v>246954370</v>
       </c>
       <c r="K3" t="s">
@@ -1314,1684 +1309,1684 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>10734720</v>
-      </c>
-      <c r="H4" s="4">
-        <v>28751500</v>
-      </c>
-      <c r="I4" s="4">
-        <v>10734720</v>
-      </c>
-      <c r="J4" s="4">
-        <v>29723190</v>
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>98134480</v>
+      </c>
+      <c r="H4">
+        <v>320580010</v>
+      </c>
+      <c r="I4">
+        <v>101154370</v>
+      </c>
+      <c r="J4">
+        <v>442811290</v>
       </c>
       <c r="K4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="M4">
-        <v>10734720</v>
+        <v>6743625</v>
       </c>
       <c r="N4">
-        <v>140</v>
+        <v>2022</v>
       </c>
       <c r="O4" s="2">
         <f>G4/$N4</f>
-        <v>76676.571428571435</v>
+        <v>48533.372898120673</v>
       </c>
       <c r="P4" s="2">
         <f>H4/$N4</f>
-        <v>205367.85714285713</v>
+        <v>158545.9990108803</v>
       </c>
       <c r="Q4" s="2">
         <f>I4/$N4</f>
-        <v>76676.571428571435</v>
+        <v>50026.889218595446</v>
       </c>
       <c r="R4" s="2">
         <f>J4/$N4</f>
-        <v>212308.5</v>
+        <v>218996.68150346191</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="4">
-        <v>20538600</v>
-      </c>
-      <c r="H5" s="4">
-        <v>60559050</v>
-      </c>
-      <c r="I5" s="4">
-        <v>21672570</v>
-      </c>
-      <c r="J5" s="4">
-        <v>64104220</v>
+      <c r="G5">
+        <v>10734720</v>
+      </c>
+      <c r="H5">
+        <v>28751500</v>
+      </c>
+      <c r="I5">
+        <v>10734720</v>
+      </c>
+      <c r="J5">
+        <v>29723190</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>10836285</v>
+        <v>10734720</v>
       </c>
       <c r="N5">
-        <v>310</v>
+        <v>140</v>
       </c>
       <c r="O5" s="2">
         <f>G5/$N5</f>
-        <v>66253.548387096773</v>
+        <v>76676.571428571435</v>
       </c>
       <c r="P5" s="2">
         <f>H5/$N5</f>
-        <v>195351.77419354839</v>
+        <v>205367.85714285713</v>
       </c>
       <c r="Q5" s="2">
         <f>I5/$N5</f>
-        <v>69911.516129032258</v>
+        <v>76676.571428571435</v>
       </c>
       <c r="R5" s="2">
         <f>J5/$N5</f>
-        <v>206787.80645161291</v>
+        <v>212308.5</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1306740</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1598200</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1306740</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1669860</v>
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>16315230</v>
+      </c>
+      <c r="H6">
+        <v>107834960</v>
+      </c>
+      <c r="I6">
+        <v>16532380</v>
+      </c>
+      <c r="J6">
+        <v>134637150</v>
       </c>
       <c r="K6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="M6">
-        <v>1306740</v>
+        <v>1033274</v>
       </c>
       <c r="N6">
-        <v>20</v>
+        <v>771</v>
       </c>
       <c r="O6" s="2">
         <f>G6/$N6</f>
-        <v>65337</v>
+        <v>21161.12840466926</v>
       </c>
       <c r="P6" s="2">
         <f>H6/$N6</f>
-        <v>79910</v>
+        <v>139863.76134889753</v>
       </c>
       <c r="Q6" s="2">
         <f>I6/$N6</f>
-        <v>65337</v>
+        <v>21442.77561608301</v>
       </c>
       <c r="R6" s="2">
         <f>J6/$N6</f>
-        <v>83493</v>
+        <v>174626.65369649805</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" s="4">
-        <v>113513570</v>
-      </c>
-      <c r="H7" s="4">
-        <v>345308130</v>
-      </c>
-      <c r="I7" s="4">
-        <v>116441700</v>
-      </c>
-      <c r="J7" s="4">
-        <v>474412700</v>
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>39472000</v>
+      </c>
+      <c r="H7">
+        <v>152570320</v>
+      </c>
+      <c r="I7">
+        <v>39657560</v>
+      </c>
+      <c r="J7">
+        <v>155108070</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="L7">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="M7">
-        <v>5544843</v>
+        <v>4957195</v>
       </c>
       <c r="N7">
-        <v>2022</v>
+        <v>902</v>
       </c>
       <c r="O7" s="2">
         <f>G7/$N7</f>
-        <v>56139.253214638971</v>
+        <v>43760.532150776053</v>
       </c>
       <c r="P7" s="2">
         <f>H7/$N7</f>
-        <v>170775.53412462908</v>
+        <v>169146.69623059867</v>
       </c>
       <c r="Q7" s="2">
         <f>I7/$N7</f>
-        <v>57587.388724035605</v>
+        <v>43966.252771618623</v>
       </c>
       <c r="R7" s="2">
         <f>J7/$N7</f>
-        <v>234625.46983184965</v>
+        <v>171960.16629711751</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="E8">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>63888340</v>
-      </c>
-      <c r="H8" s="4">
-        <v>105119390</v>
-      </c>
-      <c r="I8" s="4">
-        <v>63888340</v>
-      </c>
-      <c r="J8" s="4">
-        <v>109645400</v>
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>20315800</v>
+      </c>
+      <c r="H8">
+        <v>98055190</v>
+      </c>
+      <c r="I8">
+        <v>21367470</v>
+      </c>
+      <c r="J8">
+        <v>120644613</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="L8">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M8">
-        <v>4563453</v>
+        <v>222578</v>
       </c>
       <c r="N8">
-        <v>1330</v>
+        <v>718</v>
       </c>
       <c r="O8" s="2">
         <f>G8/$N8</f>
-        <v>48036.345864661656</v>
+        <v>28294.986072423399</v>
       </c>
       <c r="P8" s="2">
         <f>H8/$N8</f>
-        <v>79037.135338345863</v>
+        <v>136567.11699164344</v>
       </c>
       <c r="Q8" s="2">
         <f>I8/$N8</f>
-        <v>48036.345864661656</v>
+        <v>29759.707520891367</v>
       </c>
       <c r="R8" s="2">
         <f>J8/$N8</f>
-        <v>82440.150375939847</v>
+        <v>168028.70891364902</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9" s="4">
-        <v>42618000</v>
-      </c>
-      <c r="H9" s="4">
-        <v>169598060</v>
-      </c>
-      <c r="I9" s="4">
-        <v>42803560</v>
-      </c>
-      <c r="J9" s="4">
-        <v>172135810</v>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2765160</v>
+      </c>
+      <c r="H9">
+        <v>23747600</v>
+      </c>
+      <c r="I9">
+        <v>2765160</v>
+      </c>
+      <c r="J9">
+        <v>25404980</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="L9">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>4755951</v>
+        <v>2765160</v>
       </c>
       <c r="N9">
-        <v>902</v>
+        <v>160</v>
       </c>
       <c r="O9" s="2">
         <f>G9/$N9</f>
-        <v>47248.337028824833</v>
+        <v>17282.25</v>
       </c>
       <c r="P9" s="2">
         <f>H9/$N9</f>
-        <v>188024.45676274944</v>
+        <v>148422.5</v>
       </c>
       <c r="Q9" s="2">
         <f>I9/$N9</f>
-        <v>47454.057649667404</v>
+        <v>17282.25</v>
       </c>
       <c r="R9" s="2">
         <f>J9/$N9</f>
-        <v>190837.92682926828</v>
+        <v>158781.125</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="C10">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="D10">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="E10">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>57767640</v>
-      </c>
-      <c r="H10" s="4">
-        <v>169587249</v>
-      </c>
-      <c r="I10" s="4">
-        <v>60632160</v>
-      </c>
-      <c r="J10" s="4">
-        <v>196870970</v>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>20326280</v>
+      </c>
+      <c r="H10">
+        <v>128251230</v>
+      </c>
+      <c r="I10">
+        <v>20326280</v>
+      </c>
+      <c r="J10">
+        <v>148060360</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L10">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>2636181</v>
+        <v>122447</v>
       </c>
       <c r="N10">
-        <v>1413</v>
+        <v>982</v>
       </c>
       <c r="O10" s="2">
         <f>G10/$N10</f>
-        <v>40882.972399150742</v>
+        <v>20698.859470468433</v>
       </c>
       <c r="P10" s="2">
         <f>H10/$N10</f>
-        <v>120019.28450106157</v>
+        <v>130602.06720977597</v>
       </c>
       <c r="Q10" s="2">
         <f>I10/$N10</f>
-        <v>42910.233545647556</v>
+        <v>20698.859470468433</v>
       </c>
       <c r="R10" s="2">
         <f>J10/$N10</f>
-        <v>139328.35810332626</v>
+        <v>150774.29735234217</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
-        <v>59273330</v>
-      </c>
-      <c r="H11" s="4">
-        <v>123790090</v>
-      </c>
-      <c r="I11" s="4">
-        <v>59516180</v>
-      </c>
-      <c r="J11" s="4">
-        <v>123493920</v>
+      <c r="G11">
+        <v>57511380</v>
+      </c>
+      <c r="H11">
+        <v>168872979</v>
+      </c>
+      <c r="I11">
+        <v>60276180</v>
+      </c>
+      <c r="J11">
+        <v>195912890</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="L11">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="M11">
-        <v>7439523</v>
+        <v>2739826</v>
       </c>
       <c r="N11">
-        <v>1646</v>
+        <v>1413</v>
       </c>
       <c r="O11" s="2">
         <f>G11/$N11</f>
-        <v>36010.528554070472</v>
+        <v>40701.613588110406</v>
       </c>
       <c r="P11" s="2">
         <f>H11/$N11</f>
-        <v>75206.616038882144</v>
+        <v>119513.78556263269</v>
       </c>
       <c r="Q11" s="2">
         <f>I11/$N11</f>
-        <v>36158.068043742409</v>
+        <v>42658.301486199576</v>
       </c>
       <c r="R11" s="2">
         <f>J11/$N11</f>
-        <v>75026.682867557713</v>
+        <v>138650.31139419673</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4">
-        <v>20315800</v>
-      </c>
-      <c r="H12" s="4">
-        <v>98055190</v>
-      </c>
-      <c r="I12" s="4">
-        <v>21367470</v>
-      </c>
-      <c r="J12" s="4">
-        <v>120644613</v>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>4475650</v>
+      </c>
+      <c r="H12">
+        <v>31389550</v>
+      </c>
+      <c r="I12">
+        <v>4527850</v>
+      </c>
+      <c r="J12">
+        <v>28185150</v>
       </c>
       <c r="K12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L12">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>222578</v>
+        <v>2263925</v>
       </c>
       <c r="N12">
-        <v>718</v>
+        <v>214</v>
       </c>
       <c r="O12" s="2">
         <f>G12/$N12</f>
-        <v>28294.986072423399</v>
+        <v>20914.252336448597</v>
       </c>
       <c r="P12" s="2">
         <f>H12/$N12</f>
-        <v>136567.11699164344</v>
+        <v>146680.1401869159</v>
       </c>
       <c r="Q12" s="2">
         <f>I12/$N12</f>
-        <v>29759.707520891367</v>
+        <v>21158.17757009346</v>
       </c>
       <c r="R12" s="2">
         <f>J12/$N12</f>
-        <v>168028.70891364902</v>
+        <v>131706.30841121497</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="C13">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="D13">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="E13">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="F13">
-        <v>6</v>
-      </c>
-      <c r="G13" s="4">
-        <v>4863830</v>
-      </c>
-      <c r="H13" s="4">
-        <v>12525210</v>
-      </c>
-      <c r="I13" s="4">
-        <v>5039020</v>
-      </c>
-      <c r="J13" s="4">
-        <v>15094890</v>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>105608760</v>
+      </c>
+      <c r="H13">
+        <v>397487215</v>
+      </c>
+      <c r="I13">
+        <v>108176410</v>
+      </c>
+      <c r="J13">
+        <v>455317110</v>
       </c>
       <c r="K13" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="L13">
-        <v>0.19</v>
+        <v>0.02</v>
       </c>
       <c r="M13">
-        <v>193808</v>
+        <v>684661</v>
       </c>
       <c r="N13">
-        <v>170</v>
+        <v>3743</v>
       </c>
       <c r="O13" s="2">
         <f>G13/$N13</f>
-        <v>28610.764705882353</v>
+        <v>28215.004007480631</v>
       </c>
       <c r="P13" s="2">
         <f>H13/$N13</f>
-        <v>73677.705882352937</v>
+        <v>106194.82099919851</v>
       </c>
       <c r="Q13" s="2">
         <f>I13/$N13</f>
-        <v>29641.294117647059</v>
+        <v>28900.991183542614</v>
       </c>
       <c r="R13" s="2">
         <f>J13/$N13</f>
-        <v>88793.470588235301</v>
+        <v>121644.96660432807</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B14">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>167</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>167</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14" s="4">
-        <v>106219730</v>
-      </c>
-      <c r="H14" s="4">
-        <v>399523805</v>
-      </c>
-      <c r="I14" s="4">
-        <v>108831520</v>
-      </c>
-      <c r="J14" s="4">
-        <v>457500820</v>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>11514360</v>
+      </c>
+      <c r="H14">
+        <v>60148310</v>
+      </c>
+      <c r="I14">
+        <v>11806130</v>
+      </c>
+      <c r="J14">
+        <v>76880430</v>
       </c>
       <c r="K14" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="L14">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>671800</v>
+        <v>1967688</v>
       </c>
       <c r="N14">
-        <v>3743</v>
+        <v>692</v>
       </c>
       <c r="O14" s="2">
         <f>G14/$N14</f>
-        <v>28378.23403686882</v>
+        <v>16639.248554913294</v>
       </c>
       <c r="P14" s="2">
         <f>H14/$N14</f>
-        <v>106738.9273310179</v>
+        <v>86919.52312138729</v>
       </c>
       <c r="Q14" s="2">
         <f>I14/$N14</f>
-        <v>29076.01389259952</v>
+        <v>17060.881502890174</v>
       </c>
       <c r="R14" s="2">
         <f>J14/$N14</f>
-        <v>122228.37830617152</v>
+        <v>111098.887283237</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>35</v>
-      </c>
-      <c r="G15" s="4">
-        <v>17252170</v>
-      </c>
-      <c r="H15" s="4">
-        <v>110177300</v>
-      </c>
-      <c r="I15" s="4">
-        <v>16929230</v>
-      </c>
-      <c r="J15" s="4">
-        <v>135629280</v>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>7597690</v>
+      </c>
+      <c r="H15">
+        <v>35529860</v>
+      </c>
+      <c r="I15">
+        <v>7832320</v>
+      </c>
+      <c r="J15">
+        <v>40445650</v>
       </c>
       <c r="K15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="L15">
-        <v>0.67</v>
+        <v>0.1</v>
       </c>
       <c r="M15">
-        <v>995837</v>
+        <v>783232</v>
       </c>
       <c r="N15">
-        <v>771</v>
+        <v>378</v>
       </c>
       <c r="O15" s="2">
         <f>G15/$N15</f>
-        <v>22376.355382619975</v>
+        <v>20099.708994708995</v>
       </c>
       <c r="P15" s="2">
         <f>H15/$N15</f>
-        <v>142901.81582360572</v>
+        <v>93994.338624338619</v>
       </c>
       <c r="Q15" s="2">
         <f>I15/$N15</f>
-        <v>21957.496757457848</v>
+        <v>20720.423280423282</v>
       </c>
       <c r="R15" s="2">
         <f>J15/$N15</f>
-        <v>175913.46303501946</v>
+        <v>106999.07407407407</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>4475650</v>
-      </c>
-      <c r="H16" s="4">
-        <v>31389550</v>
-      </c>
-      <c r="I16" s="4">
-        <v>4527850</v>
-      </c>
-      <c r="J16" s="4">
-        <v>28185150</v>
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>4863830</v>
+      </c>
+      <c r="H16">
+        <v>12525210</v>
+      </c>
+      <c r="I16">
+        <v>5039020</v>
+      </c>
+      <c r="J16">
+        <v>15094890</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="M16">
-        <v>2263925</v>
+        <v>193808</v>
       </c>
       <c r="N16">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="O16" s="2">
         <f>G16/$N16</f>
-        <v>20914.252336448597</v>
+        <v>28610.764705882353</v>
       </c>
       <c r="P16" s="2">
         <f>H16/$N16</f>
-        <v>146680.1401869159</v>
+        <v>73677.705882352937</v>
       </c>
       <c r="Q16" s="2">
         <f>I16/$N16</f>
-        <v>21158.17757009346</v>
+        <v>29641.294117647059</v>
       </c>
       <c r="R16" s="2">
         <f>J16/$N16</f>
-        <v>131706.30841121497</v>
+        <v>88793.470588235301</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4">
-        <v>7597690</v>
-      </c>
-      <c r="H17" s="4">
-        <v>35529860</v>
-      </c>
-      <c r="I17" s="4">
-        <v>7832320</v>
-      </c>
-      <c r="J17" s="4">
-        <v>40445650</v>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1306740</v>
+      </c>
+      <c r="H17">
+        <v>1598200</v>
+      </c>
+      <c r="I17">
+        <v>1306740</v>
+      </c>
+      <c r="J17">
+        <v>1669860</v>
       </c>
       <c r="K17" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="L17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>783232</v>
+        <v>1306740</v>
       </c>
       <c r="N17">
-        <v>378</v>
+        <v>20</v>
       </c>
       <c r="O17" s="2">
         <f>G17/$N17</f>
-        <v>20099.708994708995</v>
+        <v>65337</v>
       </c>
       <c r="P17" s="2">
         <f>H17/$N17</f>
-        <v>93994.338624338619</v>
+        <v>79910</v>
       </c>
       <c r="Q17" s="2">
         <f>I17/$N17</f>
-        <v>20720.423280423282</v>
+        <v>65337</v>
       </c>
       <c r="R17" s="2">
         <f>J17/$N17</f>
-        <v>106999.07407407407</v>
+        <v>83493</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="C18">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="D18">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="E18">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>20326280</v>
-      </c>
-      <c r="H18" s="4">
-        <v>128251230</v>
-      </c>
-      <c r="I18" s="4">
-        <v>20326280</v>
-      </c>
-      <c r="J18" s="4">
-        <v>148060360</v>
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>10841720</v>
+      </c>
+      <c r="H18">
+        <v>65751870</v>
+      </c>
+      <c r="I18">
+        <v>11067560</v>
+      </c>
+      <c r="J18">
+        <v>91716770</v>
       </c>
       <c r="K18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="M18">
-        <v>122447</v>
+        <v>1383445</v>
       </c>
       <c r="N18">
-        <v>982</v>
+        <v>1117</v>
       </c>
       <c r="O18" s="2">
         <f>G18/$N18</f>
-        <v>20698.859470468433</v>
+        <v>9706.1056401074311</v>
       </c>
       <c r="P18" s="2">
         <f>H18/$N18</f>
-        <v>130602.06720977597</v>
+        <v>58864.700089525511</v>
       </c>
       <c r="Q18" s="2">
         <f>I18/$N18</f>
-        <v>20698.859470468433</v>
+        <v>9908.2900626678602</v>
       </c>
       <c r="R18" s="2">
         <f>J18/$N18</f>
-        <v>150774.29735234217</v>
+        <v>82109.910474485223</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B19">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D19">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="G19" s="4">
-        <v>19541700</v>
-      </c>
-      <c r="H19" s="4">
-        <v>63965390</v>
-      </c>
-      <c r="I19" s="4">
-        <v>19632780</v>
-      </c>
-      <c r="J19" s="4">
-        <v>77790720</v>
+      <c r="G19">
+        <v>62651110</v>
+      </c>
+      <c r="H19">
+        <v>101371440</v>
+      </c>
+      <c r="I19">
+        <v>62651110</v>
+      </c>
+      <c r="J19">
+        <v>105960930</v>
       </c>
       <c r="K19" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L19">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M19">
-        <v>755107</v>
+        <v>4819316</v>
       </c>
       <c r="N19">
-        <v>1012</v>
+        <v>1330</v>
       </c>
       <c r="O19" s="2">
         <f>G19/$N19</f>
-        <v>19309.980237154152</v>
+        <v>47106.097744360901</v>
       </c>
       <c r="P19" s="2">
         <f>H19/$N19</f>
-        <v>63206.907114624504</v>
+        <v>76219.12781954887</v>
       </c>
       <c r="Q19" s="2">
         <f>I19/$N19</f>
-        <v>19399.980237154152</v>
+        <v>47106.097744360901</v>
       </c>
       <c r="R19" s="2">
         <f>J19/$N19</f>
-        <v>76868.300395256912</v>
+        <v>79669.87218045113</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <v>2765160</v>
-      </c>
-      <c r="H20" s="4">
-        <v>23747600</v>
-      </c>
-      <c r="I20" s="4">
-        <v>2765160</v>
-      </c>
-      <c r="J20" s="4">
-        <v>25404980</v>
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>19168690</v>
+      </c>
+      <c r="H20">
+        <v>63592380</v>
+      </c>
+      <c r="I20">
+        <v>19259770</v>
+      </c>
+      <c r="J20">
+        <v>77417710</v>
       </c>
       <c r="K20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="M20">
-        <v>2765160</v>
+        <v>770391</v>
       </c>
       <c r="N20">
-        <v>160</v>
+        <v>1012</v>
       </c>
       <c r="O20" s="2">
         <f>G20/$N20</f>
-        <v>17282.25</v>
+        <v>18941.393280632412</v>
       </c>
       <c r="P20" s="2">
         <f>H20/$N20</f>
-        <v>148422.5</v>
+        <v>62838.320158102768</v>
       </c>
       <c r="Q20" s="2">
         <f>I20/$N20</f>
-        <v>17282.25</v>
+        <v>19031.393280632412</v>
       </c>
       <c r="R20" s="2">
         <f>J20/$N20</f>
-        <v>158781.125</v>
+        <v>76499.713438735183</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21">
         <v>8</v>
       </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
       <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>11514360</v>
-      </c>
-      <c r="H21" s="4">
-        <v>60148310</v>
-      </c>
-      <c r="I21" s="4">
-        <v>11806130</v>
-      </c>
-      <c r="J21" s="4">
-        <v>76880430</v>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>59273330</v>
+      </c>
+      <c r="H21">
+        <v>123790090</v>
+      </c>
+      <c r="I21">
+        <v>59516180</v>
+      </c>
+      <c r="J21">
+        <v>123493920</v>
       </c>
       <c r="K21" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="M21">
-        <v>1967688</v>
+        <v>7439523</v>
       </c>
       <c r="N21">
-        <v>692</v>
+        <v>1646</v>
       </c>
       <c r="O21" s="2">
         <f>G21/$N21</f>
-        <v>16639.248554913294</v>
+        <v>36010.528554070472</v>
       </c>
       <c r="P21" s="2">
         <f>H21/$N21</f>
-        <v>86919.52312138729</v>
+        <v>75206.616038882144</v>
       </c>
       <c r="Q21" s="2">
         <f>I21/$N21</f>
-        <v>17060.881502890174</v>
+        <v>36158.068043742409</v>
       </c>
       <c r="R21" s="2">
         <f>J21/$N21</f>
-        <v>111098.887283237</v>
+        <v>75026.682867557713</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22" s="4">
-        <v>3398760</v>
-      </c>
-      <c r="H22" s="4">
-        <v>9415230</v>
-      </c>
-      <c r="I22" s="4">
-        <v>3413300</v>
-      </c>
-      <c r="J22" s="4">
-        <v>9993880</v>
+      <c r="G22">
+        <v>9948710</v>
+      </c>
+      <c r="H22">
+        <v>50446780</v>
+      </c>
+      <c r="I22">
+        <v>11829950</v>
+      </c>
+      <c r="J22">
+        <v>64125890</v>
       </c>
       <c r="K22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>284442</v>
+        <v>1971658</v>
       </c>
       <c r="N22">
-        <v>203</v>
+        <v>1011</v>
       </c>
       <c r="O22" s="2">
         <f>G22/$N22</f>
-        <v>16742.660098522167</v>
+        <v>9840.4648862512367</v>
       </c>
       <c r="P22" s="2">
         <f>H22/$N22</f>
-        <v>46380.443349753696</v>
+        <v>49897.903066271021</v>
       </c>
       <c r="Q22" s="2">
         <f>I22/$N22</f>
-        <v>16814.285714285714</v>
+        <v>11701.236399604351</v>
       </c>
       <c r="R22" s="2">
         <f>J22/$N22</f>
-        <v>49230.93596059113</v>
+        <v>63428.18001978239</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B23">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D23">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" s="4">
-        <v>21399520</v>
-      </c>
-      <c r="H23" s="4">
-        <v>59913780</v>
-      </c>
-      <c r="I23" s="4">
-        <v>21397900</v>
-      </c>
-      <c r="J23" s="4">
-        <v>57054950</v>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>3398760</v>
+      </c>
+      <c r="H23">
+        <v>9415230</v>
+      </c>
+      <c r="I23">
+        <v>3413300</v>
+      </c>
+      <c r="J23">
+        <v>9993880</v>
       </c>
       <c r="K23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L23">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <v>891579</v>
+        <v>284442</v>
       </c>
       <c r="N23">
-        <v>1301</v>
+        <v>203</v>
       </c>
       <c r="O23" s="2">
         <f>G23/$N23</f>
-        <v>16448.516525749423</v>
+        <v>16742.660098522167</v>
       </c>
       <c r="P23" s="2">
         <f>H23/$N23</f>
-        <v>46052.098385857033</v>
+        <v>46380.443349753696</v>
       </c>
       <c r="Q23" s="2">
         <f>I23/$N23</f>
-        <v>16447.271329746349</v>
+        <v>16814.285714285714</v>
       </c>
       <c r="R23" s="2">
         <f>J23/$N23</f>
-        <v>43854.688700999228</v>
+        <v>49230.93596059113</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C24">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E24">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F24">
-        <v>3</v>
-      </c>
-      <c r="G24" s="4">
-        <v>32309420</v>
-      </c>
-      <c r="H24" s="4">
-        <v>68051680</v>
-      </c>
-      <c r="I24" s="4">
-        <v>32315040</v>
-      </c>
-      <c r="J24" s="4">
-        <v>70990390</v>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>21399520</v>
+      </c>
+      <c r="H24">
+        <v>59913780</v>
+      </c>
+      <c r="I24">
+        <v>21397900</v>
+      </c>
+      <c r="J24">
+        <v>57054950</v>
       </c>
       <c r="K24" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L24">
-        <v>0.23</v>
+        <v>0.04</v>
       </c>
       <c r="M24">
-        <v>2937731</v>
+        <v>891579</v>
       </c>
       <c r="N24">
-        <v>2175</v>
+        <v>1301</v>
       </c>
       <c r="O24" s="2">
         <f>G24/$N24</f>
-        <v>14854.905747126437</v>
+        <v>16448.516525749423</v>
       </c>
       <c r="P24" s="2">
         <f>H24/$N24</f>
-        <v>31288.128735632185</v>
+        <v>46052.098385857033</v>
       </c>
       <c r="Q24" s="2">
         <f>I24/$N24</f>
-        <v>14857.489655172414</v>
+        <v>16447.271329746349</v>
       </c>
       <c r="R24" s="2">
         <f>J24/$N24</f>
-        <v>32639.259770114943</v>
+        <v>43854.688700999228</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1695410</v>
-      </c>
-      <c r="H25" s="4">
-        <v>31643890</v>
-      </c>
-      <c r="I25" s="4">
-        <v>1695410</v>
-      </c>
-      <c r="J25" s="4">
-        <v>33900420</v>
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>63968270</v>
+      </c>
+      <c r="H25">
+        <v>168331362</v>
+      </c>
+      <c r="I25">
+        <v>63968270</v>
+      </c>
+      <c r="J25">
+        <v>174458530</v>
       </c>
       <c r="K25" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="M25">
-        <v>565137</v>
+        <v>1999008</v>
       </c>
       <c r="N25">
-        <v>115</v>
+        <v>4676</v>
       </c>
       <c r="O25" s="2">
         <f>G25/$N25</f>
-        <v>14742.695652173914</v>
+        <v>13680.12617621899</v>
       </c>
       <c r="P25" s="2">
         <f>H25/$N25</f>
-        <v>275164.26086956525</v>
+        <v>35999.008126603934</v>
       </c>
       <c r="Q25" s="2">
         <f>I25/$N25</f>
-        <v>14742.695652173914</v>
+        <v>13680.12617621899</v>
       </c>
       <c r="R25" s="2">
         <f>J25/$N25</f>
-        <v>294786.26086956525</v>
+        <v>37309.352010265182</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26" s="4">
-        <v>21300480</v>
-      </c>
-      <c r="H26" s="4">
-        <v>50135630</v>
-      </c>
-      <c r="I26" s="4">
-        <v>21603110</v>
-      </c>
-      <c r="J26" s="4">
-        <v>54035580</v>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1168410</v>
+      </c>
+      <c r="H26">
+        <v>3878690</v>
+      </c>
+      <c r="I26">
+        <v>1168410</v>
+      </c>
+      <c r="J26">
+        <v>4133820</v>
       </c>
       <c r="K26" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="L26">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>1080156</v>
+        <v>584205</v>
       </c>
       <c r="N26">
-        <v>1539</v>
+        <v>115</v>
       </c>
       <c r="O26" s="2">
         <f>G26/$N26</f>
-        <v>13840.46783625731</v>
+        <v>10160.08695652174</v>
       </c>
       <c r="P26" s="2">
         <f>H26/$N26</f>
-        <v>32576.757634827809</v>
+        <v>33727.739130434784</v>
       </c>
       <c r="Q26" s="2">
         <f>I26/$N26</f>
-        <v>14037.108512020794</v>
+        <v>10160.08695652174</v>
       </c>
       <c r="R26" s="2">
         <f>J26/$N26</f>
-        <v>35110.838206627683</v>
+        <v>35946.260869565216</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B27">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D27">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E27">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F27">
-        <v>3</v>
-      </c>
-      <c r="G27" s="4">
-        <v>65215880</v>
-      </c>
-      <c r="H27" s="4">
-        <v>170759562</v>
-      </c>
-      <c r="I27" s="4">
-        <v>65215880</v>
-      </c>
-      <c r="J27" s="4">
-        <v>177031660</v>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>20745320</v>
+      </c>
+      <c r="H27">
+        <v>47836830</v>
+      </c>
+      <c r="I27">
+        <v>20987270</v>
+      </c>
+      <c r="J27">
+        <v>50905090</v>
       </c>
       <c r="K27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L27">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M27">
-        <v>1976239</v>
+        <v>1614405</v>
       </c>
       <c r="N27">
-        <v>4676</v>
+        <v>1539</v>
       </c>
       <c r="O27" s="2">
         <f>G27/$N27</f>
-        <v>13946.937553464499</v>
+        <v>13479.740090968162</v>
       </c>
       <c r="P27" s="2">
         <f>H27/$N27</f>
-        <v>36518.298118049614</v>
+        <v>31083.060428849902</v>
       </c>
       <c r="Q27" s="2">
         <f>I27/$N27</f>
-        <v>13946.937553464499</v>
+        <v>13636.952566601689</v>
       </c>
       <c r="R27" s="2">
         <f>J27/$N27</f>
-        <v>37859.636441402909</v>
+        <v>33076.731643924628</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28" s="4">
-        <v>195360</v>
-      </c>
-      <c r="H28" s="4">
-        <v>488400</v>
-      </c>
-      <c r="I28" s="4">
-        <v>233550</v>
-      </c>
-      <c r="J28" s="4">
-        <v>583880</v>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>32309420</v>
+      </c>
+      <c r="H28">
+        <v>68051680</v>
+      </c>
+      <c r="I28">
+        <v>32315040</v>
+      </c>
+      <c r="J28">
+        <v>70990390</v>
       </c>
       <c r="K28" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="M28">
-        <v>233550</v>
+        <v>2937731</v>
       </c>
       <c r="N28">
-        <v>18</v>
+        <v>2175</v>
       </c>
       <c r="O28" s="2">
         <f>G28/$N28</f>
-        <v>10853.333333333334</v>
+        <v>14854.905747126437</v>
       </c>
       <c r="P28" s="2">
         <f>H28/$N28</f>
-        <v>27133.333333333332</v>
+        <v>31288.128735632185</v>
       </c>
       <c r="Q28" s="2">
         <f>I28/$N28</f>
-        <v>12975</v>
+        <v>14857.489655172414</v>
       </c>
       <c r="R28" s="2">
         <f>J28/$N28</f>
-        <v>32437.777777777777</v>
+        <v>32639.259770114943</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29" s="4">
-        <v>8494360</v>
-      </c>
-      <c r="H29" s="4">
-        <v>16675120</v>
-      </c>
-      <c r="I29" s="4">
-        <v>8494360</v>
-      </c>
-      <c r="J29" s="4">
-        <v>17435910</v>
+      <c r="G29">
+        <v>195360</v>
+      </c>
+      <c r="H29">
+        <v>488400</v>
+      </c>
+      <c r="I29">
+        <v>233550</v>
+      </c>
+      <c r="J29">
+        <v>583880</v>
       </c>
       <c r="K29" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>606740</v>
+        <v>233550</v>
       </c>
       <c r="N29">
-        <v>711</v>
+        <v>18</v>
       </c>
       <c r="O29" s="2">
         <f>G29/$N29</f>
-        <v>11947.060478199719</v>
+        <v>10853.333333333334</v>
       </c>
       <c r="P29" s="2">
         <f>H29/$N29</f>
-        <v>23453.052039381153</v>
+        <v>27133.333333333332</v>
       </c>
       <c r="Q29" s="2">
         <f>I29/$N29</f>
-        <v>11947.060478199719</v>
+        <v>12975</v>
       </c>
       <c r="R29" s="2">
         <f>J29/$N29</f>
-        <v>24523.080168776371</v>
+        <v>32437.777777777777</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4">
-        <v>9948710</v>
-      </c>
-      <c r="H30" s="4">
-        <v>50446780</v>
-      </c>
-      <c r="I30" s="4">
-        <v>11829950</v>
-      </c>
-      <c r="J30" s="4">
-        <v>64125890</v>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>12384600</v>
+      </c>
+      <c r="H30">
+        <v>38466770</v>
+      </c>
+      <c r="I30">
+        <v>12143330</v>
+      </c>
+      <c r="J30">
+        <v>39904950</v>
       </c>
       <c r="K30" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="M30">
-        <v>1971658</v>
+        <v>357157</v>
       </c>
       <c r="N30">
-        <v>1011</v>
+        <v>1526</v>
       </c>
       <c r="O30" s="2">
         <f>G30/$N30</f>
-        <v>9840.4648862512367</v>
+        <v>8115.7273918741812</v>
       </c>
       <c r="P30" s="2">
         <f>H30/$N30</f>
-        <v>49897.903066271021</v>
+        <v>25207.581913499344</v>
       </c>
       <c r="Q30" s="2">
         <f>I30/$N30</f>
-        <v>11701.236399604351</v>
+        <v>7957.6212319790302</v>
       </c>
       <c r="R30" s="2">
         <f>J30/$N30</f>
-        <v>63428.18001978239</v>
+        <v>26150.032765399737</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E31">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F31">
-        <v>2</v>
-      </c>
-      <c r="G31" s="4">
-        <v>10841720</v>
-      </c>
-      <c r="H31" s="4">
-        <v>65751870</v>
-      </c>
-      <c r="I31" s="4">
-        <v>11067560</v>
-      </c>
-      <c r="J31" s="4">
-        <v>91716770</v>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>8494360</v>
+      </c>
+      <c r="H31">
+        <v>16675120</v>
+      </c>
+      <c r="I31">
+        <v>8494360</v>
+      </c>
+      <c r="J31">
+        <v>17435910</v>
       </c>
       <c r="K31" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="L31">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>1383445</v>
+        <v>606740</v>
       </c>
       <c r="N31">
-        <v>1117</v>
+        <v>711</v>
       </c>
       <c r="O31" s="2">
         <f>G31/$N31</f>
-        <v>9706.1056401074311</v>
+        <v>11947.060478199719</v>
       </c>
       <c r="P31" s="2">
         <f>H31/$N31</f>
-        <v>58864.700089525511</v>
+        <v>23453.052039381153</v>
       </c>
       <c r="Q31" s="2">
         <f>I31/$N31</f>
-        <v>9908.2900626678602</v>
+        <v>11947.060478199719</v>
       </c>
       <c r="R31" s="2">
         <f>J31/$N31</f>
-        <v>82109.910474485223</v>
+        <v>24523.080168776371</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -3013,16 +3008,16 @@
       <c r="F32">
         <v>1</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32">
         <v>28199590</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32">
         <v>67290490</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32">
         <v>28203890</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32">
         <v>71628900</v>
       </c>
       <c r="K32" t="s">
@@ -3056,62 +3051,62 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B33">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="4">
-        <v>12384600</v>
-      </c>
-      <c r="H33" s="4">
-        <v>38466770</v>
-      </c>
-      <c r="I33" s="4">
-        <v>12143330</v>
-      </c>
-      <c r="J33" s="4">
-        <v>39904950</v>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>2541000</v>
+      </c>
+      <c r="H33">
+        <v>4927870</v>
+      </c>
+      <c r="I33">
+        <v>2541000</v>
+      </c>
+      <c r="J33">
+        <v>4967130</v>
       </c>
       <c r="K33" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="L33">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>357157</v>
+        <v>2541000</v>
       </c>
       <c r="N33">
-        <v>1526</v>
+        <v>310</v>
       </c>
       <c r="O33" s="2">
         <f>G33/$N33</f>
-        <v>8115.7273918741812</v>
+        <v>8196.7741935483864</v>
       </c>
       <c r="P33" s="2">
         <f>H33/$N33</f>
-        <v>25207.581913499344</v>
+        <v>15896.354838709678</v>
       </c>
       <c r="Q33" s="2">
         <f>I33/$N33</f>
-        <v>7957.6212319790302</v>
+        <v>8196.7741935483864</v>
       </c>
       <c r="R33" s="2">
         <f>J33/$N33</f>
-        <v>26150.032765399737</v>
+        <v>16023</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3119,7 +3114,7 @@
         <v>45</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3133,16 +3128,16 @@
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34">
         <v>1295460</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34">
         <v>2298420</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34">
         <v>1295460</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34">
         <v>2357740</v>
       </c>
       <c r="K34" t="s">
@@ -3175,8 +3170,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:T34">
-    <sortCondition descending="1" ref="Q2:Q34"/>
+  <sortState ref="A2:R34">
+    <sortCondition descending="1" ref="R2:R34"/>
   </sortState>
   <conditionalFormatting sqref="O2:R34">
     <cfRule type="dataBar" priority="1">

</xml_diff>